<commit_message>
updated full data prep script. adjusted target class to session number>2
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/data/df_merch_values_encoded.xlsx
+++ b/notebooks/google_merch_store/data/df_merch_values_encoded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Coding\Python\ist_dash_2024_rec\notebooks\google_merch_store\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D731D5-9719-4A50-B7D1-6408EDA474DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864086E4-5510-42D7-8431-1D640D459A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="1350" windowWidth="39435" windowHeight="18165" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-3770" windowWidth="38620" windowHeight="21100" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="event_name" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="534">
   <si>
     <t>event_name</t>
   </si>
@@ -1639,6 +1639,9 @@
   </si>
   <si>
     <t>shop.googlemerchandisestore.com</t>
+  </si>
+  <si>
+    <t>data deleted</t>
   </si>
 </sst>
 </file>
@@ -2173,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2205,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>533</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2210,7 +2213,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2226,10 +2229,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2239,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2276,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>533</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2273,7 +2284,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2281,10 +2292,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2296,7 +2315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E587B5-4742-4885-AC8D-E51D7A667EE0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>